<commit_message>
corrected cotb issue for nextbutton recognition
</commit_message>
<xml_diff>
--- a/OutputFiles/TC02_Canine_CaseFiles_Study-NCATS_WebData.xlsx
+++ b/OutputFiles/TC02_Canine_CaseFiles_Study-NCATS_WebData.xlsx
@@ -32,7 +32,7 @@
     <t>Size</t>
   </si>
   <si>
-    <t>CCB010234.pdf</t>
+    <t>CCB010045.pdf</t>
   </si>
   <si>
     <t>Pathology Report</t>
@@ -47,7 +47,7 @@
     <t>pdf</t>
   </si>
   <si>
-    <t>49.35 KB</t>
+    <t>45.27 KB</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
running only casefiledetails 2 tc
</commit_message>
<xml_diff>
--- a/OutputFiles/TC02_Canine_CaseFiles_Study-NCATS_WebData.xlsx
+++ b/OutputFiles/TC02_Canine_CaseFiles_Study-NCATS_WebData.xlsx
@@ -32,7 +32,7 @@
     <t>Size</t>
   </si>
   <si>
-    <t>CCB010045.pdf</t>
+    <t>CCB010234.pdf</t>
   </si>
   <si>
     <t>Pathology Report</t>
@@ -47,7 +47,7 @@
     <t>pdf</t>
   </si>
   <si>
-    <t>45.27 KB</t>
+    <t>49.35 KB</t>
   </si>
 </sst>
 </file>

</xml_diff>